<commit_message>
Debug for some worker to compare results
</commit_message>
<xml_diff>
--- a/Part2_Results.xlsx
+++ b/Part2_Results.xlsx
@@ -563,12 +563,8 @@
       <c r="E3" t="n">
         <v>0</v>
       </c>
-      <c r="F3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0</v>
-      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="n">
         <v>0</v>
@@ -3248,10 +3244,10 @@
         <v>0</v>
       </c>
       <c r="F65" t="n">
-        <v>-222821.4146940452</v>
+        <v>234507.5853059548</v>
       </c>
       <c r="G65" t="n">
-        <v>0</v>
+        <v>457329</v>
       </c>
       <c r="H65" t="n">
         <v>1</v>
@@ -4247,12 +4243,8 @@
       <c r="E88" t="n">
         <v>0</v>
       </c>
-      <c r="F88" t="n">
-        <v>0</v>
-      </c>
-      <c r="G88" t="n">
-        <v>0</v>
-      </c>
+      <c r="F88" t="inlineStr"/>
+      <c r="G88" t="inlineStr"/>
       <c r="H88" t="inlineStr"/>
       <c r="I88" t="n">
         <v>0</v>
@@ -4633,12 +4625,8 @@
       <c r="E97" t="n">
         <v>0</v>
       </c>
-      <c r="F97" t="n">
-        <v>0</v>
-      </c>
-      <c r="G97" t="n">
-        <v>0</v>
-      </c>
+      <c r="F97" t="inlineStr"/>
+      <c r="G97" t="inlineStr"/>
       <c r="H97" t="inlineStr"/>
       <c r="I97" t="n">
         <v>0</v>

</xml_diff>